<commit_message>
added ROC AUC curve to LR
</commit_message>
<xml_diff>
--- a/Zahin Ahmed/LR_parameter_tuning.xlsx
+++ b/Zahin Ahmed/LR_parameter_tuning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>L2_Penalty</t>
   </si>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I3"/>
+      <selection activeCell="I5" sqref="I5:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +543,135 @@
         <v>0.69</v>
       </c>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>58</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>113</v>
+      </c>
+      <c r="G4">
+        <f>F4/(F4+E4)</f>
+        <v>0.83703703703703702</v>
+      </c>
+      <c r="H4">
+        <f>C4/(C4+D4)</f>
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="I4">
+        <f>1-H4</f>
+        <v>0.30952380952380953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>113</v>
+      </c>
+      <c r="G5">
+        <f>F5/(F5+E5)</f>
+        <v>0.83703703703703702</v>
+      </c>
+      <c r="H5">
+        <f>C5/(C5+D5)</f>
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="I5">
+        <f>1-H5</f>
+        <v>0.30952380952380953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.1429</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>113</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G7" si="0">F6/(F6+E6)</f>
+        <v>0.83703703703703702</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H7" si="1">C6/(C6+D6)</f>
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="2">1-H6</f>
+        <v>0.30952380952380953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>113</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.83703703703703702</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0.30952380952380953</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>